<commit_message>
Fahrzeiten mittels API für alle Gemeinden ermittelt und in ein Excel geschrieben
</commit_message>
<xml_diff>
--- a/Ergebnisse_Fahrzeit_Distanz_Test.xlsx
+++ b/Ergebnisse_Fahrzeit_Distanz_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marina Frei\Documents\Studium\Bachelorarbeit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73DF10D-D5DE-4D08-B3ED-DA8C3F15C074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE3EDAE-CF8F-4797-8A2F-55765E0DEE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{28BD6CF5-A680-41E7-A920-37F074C277EC}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>